<commit_message>
published pre-release-files for ver5.13.3
</commit_message>
<xml_diff>
--- a/sample/ExcelMacro/kabuSTATION_API_PUSH_sample.xlsx
+++ b/sample/ExcelMacro/kabuSTATION_API_PUSH_sample.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C02107A4-8907-4DBA-87B2-3056517739B8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11190" yWindow="1500" windowWidth="20040" windowHeight="17400" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11190" yWindow="1500" windowWidth="20040" windowHeight="17400"/>
   </bookViews>
   <sheets>
     <sheet name="PUSH配信サンプル" sheetId="1" r:id="rId1"/>
@@ -29,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="220" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="115">
   <si>
     <t>売気配数量1本目</t>
     <phoneticPr fontId="1"/>
@@ -435,7 +434,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FFFF0000"/>
-        <rFont val="Yu Gothic"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -446,7 +445,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Yu Gothic"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -456,7 +455,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF00B050"/>
-        <rFont val="Yu Gothic"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -467,7 +466,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Yu Gothic"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -477,7 +476,7 @@
       <rPr>
         <sz val="11"/>
         <color rgb="FF0070C0"/>
-        <rFont val="Yu Gothic"/>
+        <rFont val="Calibri"/>
         <family val="3"/>
         <charset val="128"/>
         <scheme val="minor"/>
@@ -488,7 +487,7 @@
       <rPr>
         <sz val="11"/>
         <color theme="1"/>
-        <rFont val="Yu Gothic"/>
+        <rFont val="Calibri"/>
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
@@ -512,29 +511,32 @@
     </rPh>
     <phoneticPr fontId="2"/>
   </si>
+  <si>
+    <t>銘柄種別</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="6"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -542,7 +544,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -550,7 +552,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B050"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -558,7 +560,7 @@
     <font>
       <sz val="11"/>
       <color rgb="FF0070C0"/>
-      <name val="Yu Gothic"/>
+      <name val="Calibri"/>
       <family val="3"/>
       <charset val="128"/>
       <scheme val="minor"/>
@@ -1336,14 +1338,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:CJ3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CK3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="89" max="89" width="10.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:88">
+    <row r="1" spans="1:89">
       <c r="C1" s="1"/>
       <c r="AE1" s="2" t="s">
         <v>0</v>
@@ -1430,7 +1435,7 @@
       </c>
       <c r="CA1" s="4"/>
     </row>
-    <row r="2" spans="1:88">
+    <row r="2" spans="1:89">
       <c r="C2" s="5" t="s">
         <v>20</v>
       </c>
@@ -1689,8 +1694,11 @@
       <c r="CJ2" s="5" t="s">
         <v>105</v>
       </c>
+      <c r="CK2" s="5" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="3" spans="1:88">
+    <row r="3" spans="1:89">
       <c r="A3">
         <v>9433</v>
       </c>
@@ -1705,88 +1713,89 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{044FCBC8-A5CD-4C22-9D7E-E73B8831AFB5}">
-  <dimension ref="A1:CJ10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:CK10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="16.25" customWidth="1"/>
-    <col min="2" max="2" width="15.25" customWidth="1"/>
-    <col min="3" max="3" width="51.5" customWidth="1"/>
-    <col min="4" max="4" width="9.875" customWidth="1"/>
+    <col min="1" max="1" width="16.28515625" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" customWidth="1"/>
+    <col min="3" max="3" width="51.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
     <col min="5" max="5" width="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.5" customWidth="1"/>
+    <col min="7" max="7" width="8.42578125" customWidth="1"/>
     <col min="9" max="9" width="13" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15.125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="14" max="15" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.140625" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="11" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="26.875" bestFit="1" customWidth="1"/>
-    <col min="26" max="28" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="26" max="28" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="11" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="32" max="33" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="32" max="33" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="34" max="34" width="20" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="47" max="47" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="50" max="50" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="53" max="55" width="15.125" bestFit="1" customWidth="1"/>
-    <col min="56" max="56" width="17.25" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="47" max="47" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="50" max="50" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="51" max="51" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="52" max="52" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="53" max="55" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="56" max="56" width="17.28515625" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="11" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="59" max="60" width="13.75" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="59" max="60" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="20" bestFit="1" customWidth="1"/>
-    <col min="62" max="62" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="64" max="64" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="65" max="65" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="67" max="67" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="68" max="68" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="69" max="69" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="70" max="70" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="71" max="71" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="73" max="73" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="74" max="74" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="75" max="75" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="76" max="76" width="16.25" bestFit="1" customWidth="1"/>
-    <col min="77" max="77" width="13.75" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="17.375" bestFit="1" customWidth="1"/>
-    <col min="79" max="79" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="80" max="80" width="14.375" bestFit="1" customWidth="1"/>
-    <col min="81" max="81" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="83" max="83" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="33.25" bestFit="1" customWidth="1"/>
-    <col min="85" max="86" width="7.125" bestFit="1" customWidth="1"/>
-    <col min="87" max="87" width="5.25" bestFit="1" customWidth="1"/>
-    <col min="88" max="88" width="7.125" bestFit="1" customWidth="1"/>
+    <col min="62" max="62" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="63" max="63" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="67" max="67" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="68" max="68" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="70" max="70" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="71" max="71" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="73" max="73" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="74" max="74" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="75" max="75" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="76" max="76" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="77" max="77" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="79" max="79" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="80" max="80" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="81" max="81" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="83" max="83" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="33.28515625" bestFit="1" customWidth="1"/>
+    <col min="85" max="86" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="87" max="87" width="5.28515625" bestFit="1" customWidth="1"/>
+    <col min="88" max="88" width="7.140625" bestFit="1" customWidth="1"/>
+    <col min="89" max="89" width="10.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:88">
+    <row r="1" spans="1:89">
       <c r="C1" s="1"/>
       <c r="AE1" s="2" t="s">
         <v>0</v>
@@ -1873,7 +1882,7 @@
       </c>
       <c r="CA1" s="4"/>
     </row>
-    <row r="2" spans="1:88">
+    <row r="2" spans="1:89">
       <c r="A2" s="6" t="s">
         <v>106</v>
       </c>
@@ -2138,8 +2147,11 @@
       <c r="CJ2" s="5" t="s">
         <v>105</v>
       </c>
+      <c r="CK2" s="5" t="s">
+        <v>114</v>
+      </c>
     </row>
-    <row r="3" spans="1:88">
+    <row r="3" spans="1:89">
       <c r="A3">
         <v>9433</v>
       </c>
@@ -2150,30 +2162,30 @@
         <v>108</v>
       </c>
     </row>
-    <row r="4" spans="1:88">
+    <row r="4" spans="1:89">
       <c r="C4" s="1"/>
     </row>
-    <row r="5" spans="1:88">
+    <row r="5" spans="1:89">
       <c r="C5" s="1" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="6" spans="1:88">
+    <row r="6" spans="1:89">
       <c r="C6" s="1" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:88">
+    <row r="7" spans="1:89">
       <c r="C7" s="7" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="9" spans="1:88">
+    <row r="9" spans="1:89">
       <c r="C9" s="1" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="10" spans="1:88">
+    <row r="10" spans="1:89">
       <c r="C10" t="s">
         <v>113</v>
       </c>
@@ -2186,6 +2198,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="ドキュメント" ma:contentTypeID="0x0101008BA25A4F6E0130429890910EAB213B37" ma:contentTypeVersion="6" ma:contentTypeDescription="新しいドキュメントを作成します。" ma:contentTypeScope="" ma:versionID="f45a5ff78d1383ce4d07a654f24c1f21">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="653d2f9d-bb0b-4bd8-be4f-9b17a1a91803" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="2d800a8fa84683e6bc35547f5a6b1bb4" ns2:_="">
     <xsd:import namespace="653d2f9d-bb0b-4bd8-be4f-9b17a1a91803"/>
@@ -2343,15 +2364,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -2359,13 +2371,36 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5543294B-AF37-494C-BD09-D3ACA87EFF44}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0DECC4A-C05F-474D-83BC-9D4765993044}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B0DECC4A-C05F-474D-83BC-9D4765993044}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5543294B-AF37-494C-BD09-D3ACA87EFF44}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="653d2f9d-bb0b-4bd8-be4f-9b17a1a91803"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A941E06-94CA-4E88-A412-0117822DD61F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7A941E06-94CA-4E88-A412-0117822DD61F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>